<commit_message>
fixed cost bug and updated calibrated templates
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/brazil/model_input_variables_brazil_ip_calibrated.xlsx
+++ b/ref/ingestion/calibrated/brazil/model_input_variables_brazil_ip_calibrated.xlsx
@@ -12476,112 +12476,112 @@
         <v>1</v>
       </c>
       <c r="J96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="K96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="L96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="M96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="N96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="O96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="P96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="Q96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="R96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="S96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="T96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="U96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="V96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="W96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="X96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="Y96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="Z96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AA96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AB96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AC96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AD96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AE96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AF96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AG96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AH96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AI96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AJ96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AK96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AL96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AM96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AN96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AO96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AP96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AQ96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AR96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
       <c r="AS96">
-        <v>8175149.667</v>
+        <v>23403862.31</v>
       </c>
     </row>
     <row r="97" spans="1:45">
@@ -12598,112 +12598,112 @@
         <v>1</v>
       </c>
       <c r="J97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="K97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="L97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="M97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="N97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="O97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="P97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="Q97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="R97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="S97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="T97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="U97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="V97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="W97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="X97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="Y97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="Z97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AA97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AB97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AC97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AD97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AE97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AF97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AG97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AH97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AI97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AJ97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AK97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AL97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AM97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AN97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AO97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AP97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AQ97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AR97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
       <c r="AS97">
-        <v>10809768.12</v>
+        <v>17500919.01</v>
       </c>
     </row>
     <row r="98" spans="1:45">
@@ -12720,112 +12720,112 @@
         <v>1</v>
       </c>
       <c r="J98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="K98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="L98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="M98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="N98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="O98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="P98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="Q98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="R98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="S98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="T98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="U98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="V98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="W98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="X98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="Y98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="Z98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AA98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AB98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AC98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AD98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AE98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AF98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AG98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AH98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AI98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AJ98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AK98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AL98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AM98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AN98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AO98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AP98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AQ98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AR98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
       <c r="AS98">
-        <v>14031456.99</v>
+        <v>4452377.762</v>
       </c>
     </row>
     <row r="99" spans="1:45">
@@ -12842,112 +12842,112 @@
         <v>1</v>
       </c>
       <c r="J99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="K99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="L99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="M99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="N99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="O99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="P99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="Q99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="R99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="S99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="T99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="U99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="V99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="W99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="X99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="Y99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="Z99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AA99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AB99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AC99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AD99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AE99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AF99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AG99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AH99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AI99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AJ99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AK99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AL99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AM99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AN99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AO99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AP99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AQ99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AR99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
       <c r="AS99">
-        <v>4327799.942</v>
+        <v>296129.2898</v>
       </c>
     </row>
     <row r="100" spans="1:45">
@@ -12964,112 +12964,112 @@
         <v>1</v>
       </c>
       <c r="J100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="K100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="L100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="M100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="N100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="O100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="P100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="Q100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="R100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="S100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="T100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="U100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="V100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="W100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="X100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="Y100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="Z100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AA100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AB100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AC100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AD100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AE100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AF100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AG100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AH100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AI100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AJ100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AK100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AL100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AM100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AN100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AO100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AP100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AQ100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AR100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
       <c r="AS100">
-        <v>6288576.667</v>
+        <v>3150919.414</v>
       </c>
     </row>
     <row r="101" spans="1:45">
@@ -13086,112 +13086,112 @@
         <v>1</v>
       </c>
       <c r="J101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="K101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="L101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="M101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="N101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="O101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="P101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="Q101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="R101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="S101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="T101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="U101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="V101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="W101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="X101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="Y101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="Z101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AA101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AB101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AC101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AD101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AE101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AF101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AG101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AH101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AI101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AJ101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AK101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AL101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AM101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AN101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AO101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AP101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AQ101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AR101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
       <c r="AS101">
-        <v>7004076.659</v>
+        <v>28032991.61</v>
       </c>
     </row>
     <row r="102" spans="1:45">
@@ -13330,112 +13330,112 @@
         <v>1</v>
       </c>
       <c r="J103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="K103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="L103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="M103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="N103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="O103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="P103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="Q103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="R103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="S103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="T103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="U103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="V103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="W103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="X103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="Y103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="Z103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AA103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AB103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AC103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AD103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AE103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AF103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AG103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AH103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AI103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AJ103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AK103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AL103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AM103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AN103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AO103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AP103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AQ103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AR103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
       <c r="AS103">
-        <v>1543460.269</v>
+        <v>4939215.276</v>
       </c>
     </row>
     <row r="104" spans="1:45">
@@ -13452,112 +13452,112 @@
         <v>1</v>
       </c>
       <c r="J104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="K104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="L104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="M104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="N104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="O104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="P104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="Q104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="R104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="S104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="T104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="U104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="V104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="W104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="X104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="Y104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="Z104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AA104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AB104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AC104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AD104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AE104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AF104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AG104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AH104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AI104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AJ104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AK104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AL104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AM104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AN104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AO104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AP104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AQ104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AR104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
       <c r="AS104">
-        <v>18753016.35</v>
+        <v>4635387.512</v>
       </c>
     </row>
     <row r="105" spans="1:45">
@@ -14306,112 +14306,112 @@
         <v>1</v>
       </c>
       <c r="J111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="K111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="L111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="M111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="N111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="O111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="P111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="Q111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="R111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="S111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="T111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="U111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="V111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="W111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="X111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="Y111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="Z111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AA111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AB111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AC111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AD111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AE111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AF111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AG111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AH111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AI111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AJ111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AK111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AL111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AM111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AN111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AO111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AP111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AQ111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AR111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
       <c r="AS111">
-        <v>135234.274</v>
+        <v>281075.8373</v>
       </c>
     </row>
     <row r="112" spans="1:45">
@@ -14428,112 +14428,112 @@
         <v>1</v>
       </c>
       <c r="J112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="K112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="L112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="M112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="N112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="O112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="P112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="Q112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="R112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="S112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="T112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="U112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="V112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="W112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="X112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="Y112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="Z112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AA112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AB112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AC112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AD112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AE112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AF112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AG112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AH112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AI112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AJ112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AK112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AL112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AM112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AN112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AO112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AP112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AQ112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AR112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
       <c r="AS112">
-        <v>36651363.13</v>
+        <v>777959.6513</v>
       </c>
     </row>
     <row r="113" spans="1:45">

</xml_diff>